<commit_message>
BC goidichvu: add {GiaTriSuDung, GiaTriConLai}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoGoiDichVu/Teamplate_BaoCaoChiTietSoDuGoiDichVu.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoGoiDichVu/Teamplate_BaoCaoChiTietSoDuGoiDichVu.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Tổng cộng:</t>
   </si>
@@ -96,6 +96,12 @@
   <si>
     <t>Thành tiền chưa 
 CK</t>
+  </si>
+  <si>
+    <t>Giá trị sử dụng</t>
+  </si>
+  <si>
+    <t>Giá trị còn lại</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -292,18 +298,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,6 +330,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -642,11 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +652,7 @@
     <col min="2" max="2" width="18.5703125" style="20" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="13" customWidth="1"/>
     <col min="4" max="6" width="23.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16" style="27" customWidth="1"/>
+    <col min="7" max="7" width="16" style="23" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" style="13" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" style="13" customWidth="1"/>
@@ -663,92 +660,98 @@
     <col min="12" max="12" width="21.140625" style="3" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" style="3" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" style="18" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="30" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" style="30" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="26" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="26" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" style="5" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="5" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="18" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" style="22" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="5" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" style="22" customWidth="1"/>
-    <col min="25" max="25" width="32.85546875" style="15" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="26" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="33" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" style="26" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" style="26" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="26" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="26" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" style="26" customWidth="1"/>
+    <col min="26" max="26" width="19" style="26" customWidth="1"/>
+    <col min="27" max="27" width="32.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
       <c r="AB1" s="21"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="19"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="26"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:28" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -791,10 +794,10 @@
       <c r="N4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -803,29 +806,35 @@
       <c r="R4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="23" t="s">
+      <c r="Y4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Z4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="12"/>
       <c r="C5" s="1"/>
@@ -840,19 +849,21 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="16"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="16"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="12"/>
       <c r="C6" s="1"/>
@@ -867,19 +878,21 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="17"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="16"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="16"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="12"/>
       <c r="C7" s="1"/>
@@ -894,19 +907,21 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="16"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="16"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="12"/>
       <c r="C8" s="1"/>
@@ -921,19 +936,21 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="16"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="16"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1"/>
@@ -948,19 +965,21 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="16"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="16"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="12"/>
       <c r="C10" s="1"/>
@@ -975,19 +994,21 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="16"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="16"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="12"/>
       <c r="C11" s="1"/>
@@ -1002,19 +1023,21 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="17"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="16"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="16"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="12"/>
       <c r="C12" s="1"/>
@@ -1029,19 +1052,21 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="16"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="16"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1"/>
@@ -1056,19 +1081,21 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="16"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="16"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="12"/>
       <c r="C14" s="1"/>
@@ -1083,19 +1110,21 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="17"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="16"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="16"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="12"/>
       <c r="C15" s="1"/>
@@ -1110,19 +1139,21 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="16"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="16"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="12"/>
       <c r="C16" s="1"/>
@@ -1137,19 +1168,21 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="16"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="16"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="12"/>
       <c r="C17" s="1"/>
@@ -1164,19 +1197,21 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="16"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="16"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="12"/>
       <c r="C18" s="1"/>
@@ -1191,19 +1226,21 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="17"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="16"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="16"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="12"/>
       <c r="C19" s="1"/>
@@ -1218,19 +1255,21 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="16"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="16"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="12"/>
       <c r="C20" s="1"/>
@@ -1245,19 +1284,21 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="16"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="16"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="12"/>
       <c r="C21" s="1"/>
@@ -1272,19 +1313,21 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="17"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="16"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="16"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1"/>
@@ -1299,19 +1342,21 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="17"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="16"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="16"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="12"/>
       <c r="C23" s="1"/>
@@ -1326,19 +1371,21 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="17"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="16"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="16"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="12"/>
       <c r="C24" s="1"/>
@@ -1353,19 +1400,21 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="17"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="16"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="16"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="12"/>
       <c r="C25" s="1"/>
@@ -1380,19 +1429,21 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="17"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="16"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+      <c r="AA25" s="16"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="12"/>
       <c r="C26" s="1"/>
@@ -1407,19 +1458,21 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="17"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="16"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="16"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="12"/>
       <c r="C27" s="1"/>
@@ -1434,19 +1487,21 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="17"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="16"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27"/>
+      <c r="AA27" s="16"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="12"/>
       <c r="C28" s="1"/>
@@ -1461,40 +1516,42 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="17"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="16"/>
-    </row>
-    <row r="29" spans="1:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AA28" s="16"/>
+    </row>
+    <row r="29" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="36"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="6">
         <f>SUM(N$5:N28)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29">
+      <c r="O29" s="25"/>
+      <c r="P29" s="25">
         <f>SUM(P$5:P28)</f>
         <v>0</v>
       </c>
@@ -1503,15 +1560,15 @@
         <f>SUM(R$5:R28)</f>
         <v>0</v>
       </c>
-      <c r="S29" s="6">
+      <c r="S29" s="25">
         <f>SUM(S$5:S28)</f>
         <v>0</v>
       </c>
-      <c r="T29" s="6">
+      <c r="T29" s="25">
         <f>SUM(T$5:T28)</f>
         <v>0</v>
       </c>
-      <c r="U29" s="6">
+      <c r="U29" s="25">
         <f>SUM(U$5:U28)</f>
         <v>0</v>
       </c>
@@ -1519,7 +1576,7 @@
         <f>SUM(V$5:V28)</f>
         <v>0</v>
       </c>
-      <c r="W29" s="6">
+      <c r="W29" s="25">
         <f>SUM(W$5:W28)</f>
         <v>0</v>
       </c>
@@ -1527,12 +1584,20 @@
         <f>SUM(X$5:X28)</f>
         <v>0</v>
       </c>
-      <c r="Y29" s="6"/>
+      <c r="Y29" s="25">
+        <f>SUM(Y$5:Y28)</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="25">
+        <f>SUM(Z$5:Z28)</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A2:AA2"/>
     <mergeCell ref="A29:M29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>